<commit_message>
Some programs on BST and Strings are added
Some problems on BST from techiedelight
and some  string problems from EPI are solved
</commit_message>
<xml_diff>
--- a/Overview.xlsx
+++ b/Overview.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>ALGO NAME</t>
   </si>
@@ -93,6 +93,15 @@
   </si>
   <si>
     <t>https://www.techiedelight.com/exponential-search/</t>
+  </si>
+  <si>
+    <t>Height of a binary tree</t>
+  </si>
+  <si>
+    <t>https://www.techiedelight.com/delete-given-binary-tree-iterative-recursive/</t>
+  </si>
+  <si>
+    <t>Delete binary tree</t>
   </si>
 </sst>
 </file>
@@ -423,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,6 +580,34 @@
         <v>22</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>43908</v>
+      </c>
+      <c r="B9" s="1">
+        <v>43908</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>43908</v>
+      </c>
+      <c r="B10" s="1">
+        <v>43908</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>

</xml_diff>

<commit_message>
Added some solutions for EPI and TD
EPI problems : string problems
TD problems: LCS based problem
</commit_message>
<xml_diff>
--- a/Overview.xlsx
+++ b/Overview.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>ALGO NAME</t>
   </si>
@@ -102,6 +102,18 @@
   </si>
   <si>
     <t>Delete binary tree</t>
+  </si>
+  <si>
+    <t>leftview binary tree</t>
+  </si>
+  <si>
+    <t>level-order traversal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activity Selection </t>
+  </si>
+  <si>
+    <t>https://www.techiedelight.com/activity-selection-problem/</t>
   </si>
 </sst>
 </file>
@@ -432,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,13 +611,49 @@
         <v>43908</v>
       </c>
       <c r="B10" s="1">
-        <v>43908</v>
+        <v>43912</v>
       </c>
       <c r="C10" t="s">
         <v>25</v>
       </c>
       <c r="D10" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>43908</v>
+      </c>
+      <c r="B11" s="1">
+        <v>43912</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>43908</v>
+      </c>
+      <c r="B12" s="1">
+        <v>43912</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B13" s="1">
+        <v>43914</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>